<commit_message>
Added test for top 3 longest repairs
</commit_message>
<xml_diff>
--- a/src/test/resources/files/test_file.xlsx
+++ b/src/test/resources/files/test_file.xlsx
@@ -440,7 +440,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +546,7 @@
         <v>43863.136956018519</v>
       </c>
       <c r="E4" s="3">
-        <v>43863.213750000003</v>
+        <v>43931.213750000003</v>
       </c>
       <c r="F4" s="6">
         <v>46081503</v>
@@ -728,7 +728,7 @@
         <v>43856.02239583333</v>
       </c>
       <c r="E11" s="3">
-        <v>43856.054884259262</v>
+        <v>43857.054884259262</v>
       </c>
       <c r="F11" s="6">
         <v>46767533</v>

</xml_diff>

<commit_message>
Added implementation for top 3 recurring repairs and test for it
</commit_message>
<xml_diff>
--- a/src/test/resources/files/test_file.xlsx
+++ b/src/test/resources/files/test_file.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
   <si>
     <t>CASE ID</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>В режиме сервисного обслуживания(Supervisor)</t>
+  </si>
+  <si>
+    <t>398729</t>
+  </si>
+  <si>
+    <t>372152</t>
   </si>
 </sst>
 </file>
@@ -440,7 +446,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,8 +490,8 @@
       <c r="A2" s="1">
         <v>218728186</v>
       </c>
-      <c r="B2" s="6">
-        <v>398729</v>
+      <c r="B2" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -588,8 +594,8 @@
       <c r="A6" s="1">
         <v>218835755</v>
       </c>
-      <c r="B6" s="6">
-        <v>372152</v>
+      <c r="B6" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>13</v>
@@ -614,17 +620,17 @@
       <c r="A7" s="1">
         <v>218835839</v>
       </c>
-      <c r="B7" s="6">
-        <v>396109</v>
+      <c r="B7" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="3">
-        <v>43863.206388888888</v>
+        <v>43872.206388888888</v>
       </c>
       <c r="E7" s="3">
-        <v>43863.241539351853</v>
+        <v>43872.241539351853</v>
       </c>
       <c r="F7" s="6">
         <v>5300149446</v>
@@ -666,17 +672,17 @@
       <c r="A9" s="1">
         <v>218810128</v>
       </c>
-      <c r="B9" s="6">
-        <v>386833</v>
+      <c r="B9" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="3">
-        <v>43855.011956018519</v>
+        <v>43845.011956018519</v>
       </c>
       <c r="E9" s="3">
-        <v>43857.222569444442</v>
+        <v>43847.222569444442</v>
       </c>
       <c r="F9" s="6">
         <v>5310013039</v>

</xml_diff>